<commit_message>
I forgot I think I made additions to the heatmap
</commit_message>
<xml_diff>
--- a/GCMS_Data_Unformatted.xlsx
+++ b/GCMS_Data_Unformatted.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxtyree/Desktop/Research_Heatmap/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C1A65B82-15A0-7246-B7DA-C61C1A1763A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3221A085-2285-3348-9210-208CFB384C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16880" activeTab="1" xr2:uid="{3C1A7088-C378-1442-88AE-72D0628B8522}"/>
+    <workbookView xWindow="1500" yWindow="1300" windowWidth="27640" windowHeight="16880" activeTab="1" xr2:uid="{3C1A7088-C378-1442-88AE-72D0628B8522}"/>
   </bookViews>
   <sheets>
     <sheet name="230322_ACS_FermentationMetaboli" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="256">
   <si>
     <t>description</t>
   </si>
@@ -786,6 +799,9 @@
   </si>
   <si>
     <t>hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-methyl-1-propanol </t>
   </si>
 </sst>
 </file>
@@ -22080,11 +22096,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085F8A6E-F9B0-C740-BA1B-41B5F6A63E12}">
   <dimension ref="A1:FE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:161" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -24028,7 +24047,7 @@
     </row>
     <row r="5" spans="1:161" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -40557,5 +40576,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>